<commit_message>
Tabla caprino en proceso
</commit_message>
<xml_diff>
--- a/Documentos/EXCEL_PRUE.xlsx
+++ b/Documentos/EXCEL_PRUE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="registro" sheetId="1" r:id="rId1"/>
@@ -1418,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1491,7 +1491,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
@@ -5099,7 +5099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+    <sheetView topLeftCell="A114" workbookViewId="0">
       <selection activeCell="E148" sqref="E148"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Segundo tipo de vacuna 50%
</commit_message>
<xml_diff>
--- a/Documentos/EXCEL_PRUE.xlsx
+++ b/Documentos/EXCEL_PRUE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="registro" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="477">
   <si>
     <t>Usuario</t>
   </si>
@@ -1008,6 +1008,456 @@
   </si>
   <si>
     <t>e34</t>
+  </si>
+  <si>
+    <t>Laboratorio1</t>
+  </si>
+  <si>
+    <t>Laboratorio2</t>
+  </si>
+  <si>
+    <t>Laboratorio3</t>
+  </si>
+  <si>
+    <t>Laboratorio4</t>
+  </si>
+  <si>
+    <t>Laboratorio5</t>
+  </si>
+  <si>
+    <t>Laboratorio6</t>
+  </si>
+  <si>
+    <t>Laboratorio7</t>
+  </si>
+  <si>
+    <t>Laboratorio8</t>
+  </si>
+  <si>
+    <t>Laboratorio9</t>
+  </si>
+  <si>
+    <t>Laboratorio10</t>
+  </si>
+  <si>
+    <t>Laboratorio11</t>
+  </si>
+  <si>
+    <t>Laboratorio12</t>
+  </si>
+  <si>
+    <t>Laboratorio13</t>
+  </si>
+  <si>
+    <t>Laboratorio14</t>
+  </si>
+  <si>
+    <t>Laboratorio15</t>
+  </si>
+  <si>
+    <t>Laboratorio16</t>
+  </si>
+  <si>
+    <t>Laboratorio17</t>
+  </si>
+  <si>
+    <t>Laboratorio18</t>
+  </si>
+  <si>
+    <t>Laboratorio19</t>
+  </si>
+  <si>
+    <t>Laboratorio20</t>
+  </si>
+  <si>
+    <t>Laboratorio21</t>
+  </si>
+  <si>
+    <t>Laboratorio22</t>
+  </si>
+  <si>
+    <t>Laboratorio23</t>
+  </si>
+  <si>
+    <t>Laboratorio24</t>
+  </si>
+  <si>
+    <t>Laboratorio25</t>
+  </si>
+  <si>
+    <t>Laboratorio26</t>
+  </si>
+  <si>
+    <t>Laboratorio27</t>
+  </si>
+  <si>
+    <t>Laboratorio28</t>
+  </si>
+  <si>
+    <t>Laboratorio29</t>
+  </si>
+  <si>
+    <t>Laboratorio30</t>
+  </si>
+  <si>
+    <t>Laboratorio31</t>
+  </si>
+  <si>
+    <t>Laboratorio32</t>
+  </si>
+  <si>
+    <t>Laboratorio33</t>
+  </si>
+  <si>
+    <t>Laboratorio34</t>
+  </si>
+  <si>
+    <t>Laboratorio35</t>
+  </si>
+  <si>
+    <t>Laboratorio36</t>
+  </si>
+  <si>
+    <t>Laboratorio37</t>
+  </si>
+  <si>
+    <t>Laboratorio38</t>
+  </si>
+  <si>
+    <t>Laboratorio39</t>
+  </si>
+  <si>
+    <t>Laboratorio40</t>
+  </si>
+  <si>
+    <t>Laboratorio41</t>
+  </si>
+  <si>
+    <t>Laboratorio42</t>
+  </si>
+  <si>
+    <t>Laboratorio43</t>
+  </si>
+  <si>
+    <t>Laboratorio44</t>
+  </si>
+  <si>
+    <t>Laboratorio45</t>
+  </si>
+  <si>
+    <t>Laboratorio46</t>
+  </si>
+  <si>
+    <t>Laboratorio47</t>
+  </si>
+  <si>
+    <t>Laboratorio48</t>
+  </si>
+  <si>
+    <t>Laboratorio49</t>
+  </si>
+  <si>
+    <t>Laboratorio50</t>
+  </si>
+  <si>
+    <t>Laboratorio51</t>
+  </si>
+  <si>
+    <t>Laboratorio52</t>
+  </si>
+  <si>
+    <t>Laboratorio53</t>
+  </si>
+  <si>
+    <t>Laboratorio54</t>
+  </si>
+  <si>
+    <t>Laboratorio55</t>
+  </si>
+  <si>
+    <t>Laboratorio56</t>
+  </si>
+  <si>
+    <t>Laboratorio57</t>
+  </si>
+  <si>
+    <t>Laboratorio58</t>
+  </si>
+  <si>
+    <t>Laboratorio59</t>
+  </si>
+  <si>
+    <t>Laboratorio60</t>
+  </si>
+  <si>
+    <t>Laboratorio61</t>
+  </si>
+  <si>
+    <t>Laboratorio62</t>
+  </si>
+  <si>
+    <t>Laboratorio63</t>
+  </si>
+  <si>
+    <t>Laboratorio64</t>
+  </si>
+  <si>
+    <t>Laboratorio65</t>
+  </si>
+  <si>
+    <t>Laboratorio66</t>
+  </si>
+  <si>
+    <t>Laboratorio67</t>
+  </si>
+  <si>
+    <t>Laboratorio68</t>
+  </si>
+  <si>
+    <t>Laboratorio69</t>
+  </si>
+  <si>
+    <t>Laboratorio70</t>
+  </si>
+  <si>
+    <t>Laboratorio71</t>
+  </si>
+  <si>
+    <t>Laboratorio72</t>
+  </si>
+  <si>
+    <t>Laboratorio73</t>
+  </si>
+  <si>
+    <t>Laboratorio74</t>
+  </si>
+  <si>
+    <t>Laboratorio75</t>
+  </si>
+  <si>
+    <t>Laboratorio76</t>
+  </si>
+  <si>
+    <t>Laboratorio77</t>
+  </si>
+  <si>
+    <t>Laboratorio78</t>
+  </si>
+  <si>
+    <t>Laboratorio79</t>
+  </si>
+  <si>
+    <t>Laboratorio80</t>
+  </si>
+  <si>
+    <t>Laboratorio81</t>
+  </si>
+  <si>
+    <t>Laboratorio82</t>
+  </si>
+  <si>
+    <t>Laboratorio83</t>
+  </si>
+  <si>
+    <t>Laboratorio84</t>
+  </si>
+  <si>
+    <t>Laboratorio85</t>
+  </si>
+  <si>
+    <t>Laboratorio86</t>
+  </si>
+  <si>
+    <t>Laboratorio87</t>
+  </si>
+  <si>
+    <t>Laboratorio88</t>
+  </si>
+  <si>
+    <t>Laboratorio89</t>
+  </si>
+  <si>
+    <t>Laboratorio90</t>
+  </si>
+  <si>
+    <t>Laboratorio91</t>
+  </si>
+  <si>
+    <t>Laboratorio92</t>
+  </si>
+  <si>
+    <t>Laboratorio93</t>
+  </si>
+  <si>
+    <t>Laboratorio94</t>
+  </si>
+  <si>
+    <t>Laboratorio95</t>
+  </si>
+  <si>
+    <t>Laboratorio96</t>
+  </si>
+  <si>
+    <t>Laboratorio97</t>
+  </si>
+  <si>
+    <t>Laboratorio98</t>
+  </si>
+  <si>
+    <t>Laboratorio99</t>
+  </si>
+  <si>
+    <t>Laboratorio100</t>
+  </si>
+  <si>
+    <t>Laboratorio101</t>
+  </si>
+  <si>
+    <t>Laboratorio102</t>
+  </si>
+  <si>
+    <t>Laboratorio103</t>
+  </si>
+  <si>
+    <t>Laboratorio104</t>
+  </si>
+  <si>
+    <t>Laboratorio105</t>
+  </si>
+  <si>
+    <t>Laboratorio106</t>
+  </si>
+  <si>
+    <t>Laboratorio107</t>
+  </si>
+  <si>
+    <t>Laboratorio108</t>
+  </si>
+  <si>
+    <t>Laboratorio109</t>
+  </si>
+  <si>
+    <t>Laboratorio110</t>
+  </si>
+  <si>
+    <t>Laboratorio111</t>
+  </si>
+  <si>
+    <t>Laboratorio112</t>
+  </si>
+  <si>
+    <t>Laboratorio113</t>
+  </si>
+  <si>
+    <t>Laboratorio114</t>
+  </si>
+  <si>
+    <t>Laboratorio115</t>
+  </si>
+  <si>
+    <t>Laboratorio116</t>
+  </si>
+  <si>
+    <t>Laboratorio117</t>
+  </si>
+  <si>
+    <t>Laboratorio118</t>
+  </si>
+  <si>
+    <t>Laboratorio119</t>
+  </si>
+  <si>
+    <t>Laboratorio120</t>
+  </si>
+  <si>
+    <t>Laboratorio121</t>
+  </si>
+  <si>
+    <t>Laboratorio122</t>
+  </si>
+  <si>
+    <t>Laboratorio123</t>
+  </si>
+  <si>
+    <t>Laboratorio124</t>
+  </si>
+  <si>
+    <t>Laboratorio125</t>
+  </si>
+  <si>
+    <t>Laboratorio126</t>
+  </si>
+  <si>
+    <t>Laboratorio127</t>
+  </si>
+  <si>
+    <t>Laboratorio128</t>
+  </si>
+  <si>
+    <t>Laboratorio129</t>
+  </si>
+  <si>
+    <t>Laboratorio130</t>
+  </si>
+  <si>
+    <t>Laboratorio131</t>
+  </si>
+  <si>
+    <t>Laboratorio132</t>
+  </si>
+  <si>
+    <t>Laboratorio133</t>
+  </si>
+  <si>
+    <t>Laboratorio134</t>
+  </si>
+  <si>
+    <t>Laboratorio135</t>
+  </si>
+  <si>
+    <t>Laboratorio136</t>
+  </si>
+  <si>
+    <t>Laboratorio137</t>
+  </si>
+  <si>
+    <t>Laboratorio138</t>
+  </si>
+  <si>
+    <t>Laboratorio139</t>
+  </si>
+  <si>
+    <t>Laboratorio140</t>
+  </si>
+  <si>
+    <t>Laboratorio141</t>
+  </si>
+  <si>
+    <t>Laboratorio142</t>
+  </si>
+  <si>
+    <t>Laboratorio143</t>
+  </si>
+  <si>
+    <t>Laboratorio144</t>
+  </si>
+  <si>
+    <t>Laboratorio145</t>
+  </si>
+  <si>
+    <t>Laboratorio146</t>
+  </si>
+  <si>
+    <t>Laboratorio147</t>
+  </si>
+  <si>
+    <t>Laboratorio148</t>
+  </si>
+  <si>
+    <t>Laboratorio149</t>
+  </si>
+  <si>
+    <t>Laboratorio150</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1102,6 +1552,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1418,7 +1869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1553,7 +2004,7 @@
         <v>17</v>
       </c>
       <c r="H4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="5">
         <v>2</v>
@@ -5097,18 +5548,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C153"/>
+  <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="E148" sqref="E148"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="F119" sqref="F119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4">
         <v>1</v>
       </c>
@@ -5118,8 +5570,11 @@
       <c r="C1" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>2</v>
       </c>
@@ -5129,8 +5584,11 @@
       <c r="C2" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -5140,8 +5598,11 @@
       <c r="C3" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -5151,8 +5612,11 @@
       <c r="C4" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -5162,8 +5626,11 @@
       <c r="C5" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -5173,8 +5640,11 @@
       <c r="C6" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>2</v>
       </c>
@@ -5184,8 +5654,11 @@
       <c r="C7" s="4" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -5195,8 +5668,11 @@
       <c r="C8" s="4" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>2</v>
       </c>
@@ -5206,8 +5682,11 @@
       <c r="C9" s="4" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -5217,8 +5696,11 @@
       <c r="C10" s="4" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -5228,8 +5710,11 @@
       <c r="C11" s="4" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>2</v>
       </c>
@@ -5239,8 +5724,11 @@
       <c r="C12" s="4" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>1</v>
       </c>
@@ -5250,8 +5738,11 @@
       <c r="C13" s="4" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>2</v>
       </c>
@@ -5261,8 +5752,11 @@
       <c r="C14" s="4" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>1</v>
       </c>
@@ -5272,8 +5766,11 @@
       <c r="C15" s="4" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>1</v>
       </c>
@@ -5283,8 +5780,11 @@
       <c r="C16" s="4" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>2</v>
       </c>
@@ -5294,8 +5794,11 @@
       <c r="C17" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>1</v>
       </c>
@@ -5305,8 +5808,11 @@
       <c r="C18" s="4" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>2</v>
       </c>
@@ -5316,8 +5822,11 @@
       <c r="C19" s="4" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>1</v>
       </c>
@@ -5327,8 +5836,11 @@
       <c r="C20" s="4" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>1</v>
       </c>
@@ -5338,8 +5850,11 @@
       <c r="C21" s="4" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>2</v>
       </c>
@@ -5349,8 +5864,11 @@
       <c r="C22" s="4" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>1</v>
       </c>
@@ -5360,8 +5878,11 @@
       <c r="C23" s="4" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>2</v>
       </c>
@@ -5371,8 +5892,11 @@
       <c r="C24" s="4" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>1</v>
       </c>
@@ -5382,8 +5906,11 @@
       <c r="C25" s="4" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>1</v>
       </c>
@@ -5393,8 +5920,11 @@
       <c r="C26" s="4" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>2</v>
       </c>
@@ -5404,8 +5934,11 @@
       <c r="C27" s="4" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>1</v>
       </c>
@@ -5415,8 +5948,11 @@
       <c r="C28" s="4" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>2</v>
       </c>
@@ -5426,8 +5962,11 @@
       <c r="C29" s="4" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>1</v>
       </c>
@@ -5437,8 +5976,11 @@
       <c r="C30" s="4" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>1</v>
       </c>
@@ -5448,8 +5990,11 @@
       <c r="C31" s="4" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>2</v>
       </c>
@@ -5459,8 +6004,11 @@
       <c r="C32" s="4" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>1</v>
       </c>
@@ -5470,8 +6018,11 @@
       <c r="C33" s="4" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>2</v>
       </c>
@@ -5481,8 +6032,11 @@
       <c r="C34" s="4" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>1</v>
       </c>
@@ -5492,8 +6046,11 @@
       <c r="C35" s="4" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>1</v>
       </c>
@@ -5503,8 +6060,11 @@
       <c r="C36" s="4" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>2</v>
       </c>
@@ -5514,8 +6074,11 @@
       <c r="C37" s="4" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>1</v>
       </c>
@@ -5525,8 +6088,11 @@
       <c r="C38" s="4" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>2</v>
       </c>
@@ -5536,8 +6102,11 @@
       <c r="C39" s="4" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>1</v>
       </c>
@@ -5547,8 +6116,11 @@
       <c r="C40" s="4" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>1</v>
       </c>
@@ -5558,8 +6130,11 @@
       <c r="C41" s="4" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>2</v>
       </c>
@@ -5569,8 +6144,11 @@
       <c r="C42" s="4" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>1</v>
       </c>
@@ -5580,8 +6158,11 @@
       <c r="C43" s="4" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>2</v>
       </c>
@@ -5591,8 +6172,11 @@
       <c r="C44" s="4" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>1</v>
       </c>
@@ -5602,8 +6186,11 @@
       <c r="C45" s="4" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>1</v>
       </c>
@@ -5613,8 +6200,11 @@
       <c r="C46" s="4" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>2</v>
       </c>
@@ -5624,8 +6214,11 @@
       <c r="C47" s="4" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>1</v>
       </c>
@@ -5635,8 +6228,11 @@
       <c r="C48" s="4" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>2</v>
       </c>
@@ -5646,8 +6242,11 @@
       <c r="C49" s="4" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>1</v>
       </c>
@@ -5657,8 +6256,11 @@
       <c r="C50" s="4" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>1</v>
       </c>
@@ -5668,8 +6270,11 @@
       <c r="C51" s="4" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>2</v>
       </c>
@@ -5679,8 +6284,11 @@
       <c r="C52" s="4" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>1</v>
       </c>
@@ -5690,8 +6298,11 @@
       <c r="C53" s="4" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>2</v>
       </c>
@@ -5701,8 +6312,11 @@
       <c r="C54" s="4" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>1</v>
       </c>
@@ -5712,8 +6326,11 @@
       <c r="C55" s="4" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>1</v>
       </c>
@@ -5723,8 +6340,11 @@
       <c r="C56" s="4" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>2</v>
       </c>
@@ -5734,8 +6354,11 @@
       <c r="C57" s="4" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>1</v>
       </c>
@@ -5745,8 +6368,11 @@
       <c r="C58" s="4" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>2</v>
       </c>
@@ -5756,8 +6382,11 @@
       <c r="C59" s="4" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>1</v>
       </c>
@@ -5767,8 +6396,11 @@
       <c r="C60" s="4" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>1</v>
       </c>
@@ -5778,8 +6410,11 @@
       <c r="C61" s="4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>2</v>
       </c>
@@ -5789,8 +6424,11 @@
       <c r="C62" s="4" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>1</v>
       </c>
@@ -5800,8 +6438,11 @@
       <c r="C63" s="4" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>2</v>
       </c>
@@ -5811,8 +6452,11 @@
       <c r="C64" s="4" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>1</v>
       </c>
@@ -5822,8 +6466,11 @@
       <c r="C65" s="4" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>1</v>
       </c>
@@ -5833,8 +6480,11 @@
       <c r="C66" s="4" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>2</v>
       </c>
@@ -5844,8 +6494,11 @@
       <c r="C67" s="4" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>1</v>
       </c>
@@ -5855,8 +6508,11 @@
       <c r="C68" s="4" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D68" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>2</v>
       </c>
@@ -5866,8 +6522,11 @@
       <c r="C69" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D69" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>1</v>
       </c>
@@ -5877,8 +6536,11 @@
       <c r="C70" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D70" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>1</v>
       </c>
@@ -5888,8 +6550,11 @@
       <c r="C71" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D71" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>2</v>
       </c>
@@ -5899,8 +6564,11 @@
       <c r="C72" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D72" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>1</v>
       </c>
@@ -5910,8 +6578,11 @@
       <c r="C73" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D73" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>2</v>
       </c>
@@ -5921,8 +6592,11 @@
       <c r="C74" s="4" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D74" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>1</v>
       </c>
@@ -5932,8 +6606,11 @@
       <c r="C75" s="4" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>1</v>
       </c>
@@ -5943,8 +6620,11 @@
       <c r="C76" s="4" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>2</v>
       </c>
@@ -5954,8 +6634,11 @@
       <c r="C77" s="4" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D77" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
         <v>1</v>
       </c>
@@ -5965,8 +6648,11 @@
       <c r="C78" s="4" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D78" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
         <v>2</v>
       </c>
@@ -5976,8 +6662,11 @@
       <c r="C79" s="4" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
         <v>1</v>
       </c>
@@ -5987,8 +6676,11 @@
       <c r="C80" s="4" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>1</v>
       </c>
@@ -5998,8 +6690,11 @@
       <c r="C81" s="4" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>2</v>
       </c>
@@ -6009,8 +6704,11 @@
       <c r="C82" s="4" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
         <v>1</v>
       </c>
@@ -6020,8 +6718,11 @@
       <c r="C83" s="4" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
         <v>2</v>
       </c>
@@ -6031,8 +6732,11 @@
       <c r="C84" s="4" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
         <v>1</v>
       </c>
@@ -6042,8 +6746,11 @@
       <c r="C85" s="4" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
         <v>1</v>
       </c>
@@ -6053,8 +6760,11 @@
       <c r="C86" s="4" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
         <v>2</v>
       </c>
@@ -6064,8 +6774,11 @@
       <c r="C87" s="4" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D87" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
         <v>1</v>
       </c>
@@ -6075,8 +6788,11 @@
       <c r="C88" s="4" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D88" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
         <v>2</v>
       </c>
@@ -6086,8 +6802,11 @@
       <c r="C89" s="4" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>1</v>
       </c>
@@ -6097,8 +6816,11 @@
       <c r="C90" s="4" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D90" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
         <v>1</v>
       </c>
@@ -6108,8 +6830,11 @@
       <c r="C91" s="4" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D91" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
         <v>2</v>
       </c>
@@ -6119,8 +6844,11 @@
       <c r="C92" s="4" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D92" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
         <v>1</v>
       </c>
@@ -6130,8 +6858,11 @@
       <c r="C93" s="4" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D93" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
         <v>2</v>
       </c>
@@ -6141,8 +6872,11 @@
       <c r="C94" s="4" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D94" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
         <v>1</v>
       </c>
@@ -6152,8 +6886,11 @@
       <c r="C95" s="4" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D95" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
         <v>1</v>
       </c>
@@ -6163,8 +6900,11 @@
       <c r="C96" s="4" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D96" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
         <v>2</v>
       </c>
@@ -6174,8 +6914,11 @@
       <c r="C97" s="4" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D97" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
         <v>1</v>
       </c>
@@ -6185,8 +6928,11 @@
       <c r="C98" s="4" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D98" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
         <v>2</v>
       </c>
@@ -6196,8 +6942,11 @@
       <c r="C99" s="4" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D99" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
         <v>1</v>
       </c>
@@ -6207,8 +6956,11 @@
       <c r="C100" s="4" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D100" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
         <v>1</v>
       </c>
@@ -6218,8 +6970,11 @@
       <c r="C101" s="4" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D101" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
         <v>1</v>
       </c>
@@ -6229,8 +6984,11 @@
       <c r="C102" s="4" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D102" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
         <v>2</v>
       </c>
@@ -6240,8 +6998,11 @@
       <c r="C103" s="4" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D103" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
         <v>1</v>
       </c>
@@ -6251,8 +7012,11 @@
       <c r="C104" s="4" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D104" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
         <v>2</v>
       </c>
@@ -6262,8 +7026,11 @@
       <c r="C105" s="4" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D105" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
         <v>1</v>
       </c>
@@ -6273,8 +7040,11 @@
       <c r="C106" s="4" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D106" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="4">
         <v>1</v>
       </c>
@@ -6284,8 +7054,11 @@
       <c r="C107" s="4" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D107" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
         <v>2</v>
       </c>
@@ -6295,8 +7068,11 @@
       <c r="C108" s="4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D108" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="4">
         <v>1</v>
       </c>
@@ -6306,8 +7082,11 @@
       <c r="C109" s="4" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D109" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="4">
         <v>2</v>
       </c>
@@ -6317,8 +7096,11 @@
       <c r="C110" s="4" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D110" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="4">
         <v>1</v>
       </c>
@@ -6328,8 +7110,11 @@
       <c r="C111" s="4" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D111" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="4">
         <v>1</v>
       </c>
@@ -6339,8 +7124,11 @@
       <c r="C112" s="4" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D112" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="4">
         <v>2</v>
       </c>
@@ -6350,8 +7138,11 @@
       <c r="C113" s="4" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D113" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="4">
         <v>1</v>
       </c>
@@ -6361,8 +7152,11 @@
       <c r="C114" s="4" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D114" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="4">
         <v>2</v>
       </c>
@@ -6372,8 +7166,11 @@
       <c r="C115" s="4" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D115" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="4">
         <v>1</v>
       </c>
@@ -6383,8 +7180,11 @@
       <c r="C116" s="4" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D116" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="4">
         <v>1</v>
       </c>
@@ -6394,8 +7194,11 @@
       <c r="C117" s="4" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D117" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="4">
         <v>2</v>
       </c>
@@ -6405,8 +7208,11 @@
       <c r="C118" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D118" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="4">
         <v>1</v>
       </c>
@@ -6416,8 +7222,12 @@
       <c r="C119" s="4" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D119" t="s">
+        <v>445</v>
+      </c>
+      <c r="F119" s="11"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="4">
         <v>2</v>
       </c>
@@ -6427,8 +7237,11 @@
       <c r="C120" s="4" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D120" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="4">
         <v>1</v>
       </c>
@@ -6438,8 +7251,11 @@
       <c r="C121" s="4" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D121" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="4">
         <v>1</v>
       </c>
@@ -6449,8 +7265,11 @@
       <c r="C122" s="4" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D122" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="4">
         <v>2</v>
       </c>
@@ -6460,8 +7279,11 @@
       <c r="C123" s="4" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D123" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="4">
         <v>1</v>
       </c>
@@ -6471,8 +7293,11 @@
       <c r="C124" s="4" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D124" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="4">
         <v>2</v>
       </c>
@@ -6482,8 +7307,11 @@
       <c r="C125" s="4" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D125" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="4">
         <v>1</v>
       </c>
@@ -6493,8 +7321,11 @@
       <c r="C126" s="4" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D126" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="4">
         <v>1</v>
       </c>
@@ -6504,8 +7335,11 @@
       <c r="C127" s="4" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D127" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="4">
         <v>1</v>
       </c>
@@ -6515,8 +7349,11 @@
       <c r="C128" s="4" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D128" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="4">
         <v>2</v>
       </c>
@@ -6526,8 +7363,11 @@
       <c r="C129" s="4" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D129" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="4">
         <v>1</v>
       </c>
@@ -6537,8 +7377,11 @@
       <c r="C130" s="4" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D130" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="4">
         <v>2</v>
       </c>
@@ -6548,8 +7391,11 @@
       <c r="C131" s="4" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D131" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="4">
         <v>1</v>
       </c>
@@ -6559,8 +7405,11 @@
       <c r="C132" s="4" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D132" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="4">
         <v>1</v>
       </c>
@@ -6570,8 +7419,11 @@
       <c r="C133" s="4" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D133" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="4">
         <v>2</v>
       </c>
@@ -6581,8 +7433,11 @@
       <c r="C134" s="4" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D134" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="4">
         <v>1</v>
       </c>
@@ -6592,8 +7447,11 @@
       <c r="C135" s="4" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D135" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="4">
         <v>2</v>
       </c>
@@ -6603,8 +7461,11 @@
       <c r="C136" s="4" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D136" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="4">
         <v>1</v>
       </c>
@@ -6614,8 +7475,11 @@
       <c r="C137" s="4" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D137" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="4">
         <v>1</v>
       </c>
@@ -6625,8 +7489,11 @@
       <c r="C138" s="4" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D138" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="4">
         <v>2</v>
       </c>
@@ -6636,8 +7503,11 @@
       <c r="C139" s="4" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D139" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="4">
         <v>1</v>
       </c>
@@ -6647,8 +7517,11 @@
       <c r="C140" s="4" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D140" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="4">
         <v>2</v>
       </c>
@@ -6658,8 +7531,11 @@
       <c r="C141" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D141" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="4">
         <v>1</v>
       </c>
@@ -6669,8 +7545,11 @@
       <c r="C142" s="4" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D142" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="4">
         <v>1</v>
       </c>
@@ -6680,8 +7559,11 @@
       <c r="C143" s="4" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D143" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="4">
         <v>2</v>
       </c>
@@ -6691,8 +7573,11 @@
       <c r="C144" s="4" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D144" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="4">
         <v>1</v>
       </c>
@@ -6702,8 +7587,11 @@
       <c r="C145" s="4" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D145" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="4">
         <v>2</v>
       </c>
@@ -6713,8 +7601,11 @@
       <c r="C146" s="4" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D146" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="4">
         <v>1</v>
       </c>
@@ -6724,8 +7615,11 @@
       <c r="C147" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D147" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="4">
         <v>1</v>
       </c>
@@ -6735,8 +7629,11 @@
       <c r="C148" s="4" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D148" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="4">
         <v>2</v>
       </c>
@@ -6746,8 +7643,11 @@
       <c r="C149" s="4" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D149" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="4">
         <v>1</v>
       </c>
@@ -6757,23 +7657,27 @@
       <c r="C150" s="4" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D150" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="4"/>
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="4"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="4"/>
       <c r="B153" s="4"/>
       <c r="C153" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adefoc base Antirrabica ok
</commit_message>
<xml_diff>
--- a/Documentos/EXCEL_PRUE.xlsx
+++ b/Documentos/EXCEL_PRUE.xlsx
@@ -1464,7 +1464,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1474,6 +1474,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1526,7 +1534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1553,6 +1561,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1870,7 +1881,7 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2004,10 +2015,10 @@
         <v>17</v>
       </c>
       <c r="H4" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" s="5">
         <v>2</v>
@@ -2027,13 +2038,13 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>13</v>
@@ -2051,10 +2062,10 @@
         <v>1</v>
       </c>
       <c r="I5" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J5" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>24</v>
@@ -2094,7 +2105,7 @@
       <c r="H6" s="4">
         <v>1</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="12">
         <v>1</v>
       </c>
       <c r="J6" s="5">

</xml_diff>